<commit_message>
Updates based on Kea's email
</commit_message>
<xml_diff>
--- a/Planning/planning_2017/data/treegarden_2017add.xlsx
+++ b/Planning/planning_2017/data/treegarden_2017add.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="0" windowWidth="22240" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="1520" yWindow="20" windowWidth="22240" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="addtogarden" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="171">
   <si>
     <t>id</t>
   </si>
@@ -336,13 +336,211 @@
   </si>
   <si>
     <t xml:space="preserve">I included plants I thought we needed (see R script) as well as upped the replicates of some species and decided to add 2 new species. </t>
+  </si>
+  <si>
+    <t>Updates by Lizzie on 9 May 2017:</t>
+  </si>
+  <si>
+    <t>Going through this email from Kea:</t>
+  </si>
+  <si>
+    <t>These are the plants that I think are big enough for transplanting this year, from GH 5:</t>
+  </si>
+  <si>
+    <t>6 DIELON GR</t>
+  </si>
+  <si>
+    <t>4 DIELON WM</t>
+  </si>
+  <si>
+    <t>3 BETPOP GR </t>
+  </si>
+  <si>
+    <t>1 KALANG WM</t>
+  </si>
+  <si>
+    <t>1 KALANG HF</t>
+  </si>
+  <si>
+    <t>1 SPITOM GR</t>
+  </si>
+  <si>
+    <t>I did another inventory in the common garden area, and the following plants are either dead or damaged:</t>
+  </si>
+  <si>
+    <t>Plot 5: 1 ALNINC GR - this plant is alive and sprouting from suckers, but its main stem was broken off</t>
+  </si>
+  <si>
+    <t>Plot 6: 1 ALNINC GR - same as plot 5 - alive but broken; also 2 dead ACEPENs - an HF and a WM</t>
+  </si>
+  <si>
+    <t>Plot 8: 1 MYRGAL WM</t>
+  </si>
+  <si>
+    <t>Plot 9: 2 ACEPEN WMs and 1 BETALL SH</t>
+  </si>
+  <si>
+    <t>Plot 10: 2 SAMRAC GRs, 1 DIELON GR, and 1 SORAME SH - this plant is alive but has a broken main stem - this might not matter for shrubs</t>
+  </si>
+  <si>
+    <t>I also remembered that there are some new (last season) plants in the raised beds - I assume these will be moving into the common garden:</t>
+  </si>
+  <si>
+    <t>3 BETPAP GR</t>
+  </si>
+  <si>
+    <t>1 BETPAP SH</t>
+  </si>
+  <si>
+    <t>1 ACESPI SH</t>
+  </si>
+  <si>
+    <t>1 ACESPI WM</t>
+  </si>
+  <si>
+    <t>1 SPIALB WM</t>
+  </si>
+  <si>
+    <t>1 SPIALB SH</t>
+  </si>
+  <si>
+    <t>2 SORAME SH</t>
+  </si>
+  <si>
+    <t>2 AMECAN SH</t>
+  </si>
+  <si>
+    <t>My notes on this:</t>
+  </si>
+  <si>
+    <t>What we have in GH 5 and whether we need it:</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>some DIELON GR also available in GH5</t>
+  </si>
+  <si>
+    <t>DIELONXX_WM</t>
+  </si>
+  <si>
+    <t>in GH5, according to Kea's email</t>
+  </si>
+  <si>
+    <t>Use all! Have added to 'addtogarden' tab</t>
+  </si>
+  <si>
+    <t>Not growing this species</t>
+  </si>
+  <si>
+    <t>What we need to add because it's dead or damaged:</t>
+  </si>
+  <si>
+    <t>ALNIC GR (plot 5)</t>
+  </si>
+  <si>
+    <t>ALNIC GR (plot 6)</t>
+  </si>
+  <si>
+    <t>ACEPEN_HF (plot 6)</t>
+  </si>
+  <si>
+    <t>ACEPEN_WM (plot 6)</t>
+  </si>
+  <si>
+    <t>Use one to replace dead one in plot 10; Have noted in 'addtogarden' tab</t>
+  </si>
+  <si>
+    <t>MYRGAL_WM (plot 8)</t>
+  </si>
+  <si>
+    <t>ACEPEN_WM (plot 9)</t>
+  </si>
+  <si>
+    <t>BETALL_SH (plot 9)</t>
+  </si>
+  <si>
+    <t>SAMRAC_GR (plot 10)</t>
+  </si>
+  <si>
+    <t>DIELON_GR (plot 10)</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 5</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 6</t>
+  </si>
+  <si>
+    <t>ALNINC08_GR</t>
+  </si>
+  <si>
+    <t>ALNINC10_GR</t>
+  </si>
+  <si>
+    <t>just adding an extra one since 2 already died!</t>
+  </si>
+  <si>
+    <t>had added replacement one in 'addtogarden' tab</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 9</t>
+  </si>
+  <si>
+    <t>ACEPEN05_WM</t>
+  </si>
+  <si>
+    <t>ACEPEN</t>
+  </si>
+  <si>
+    <t>we do not have this to add I don't think ….</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 8</t>
+  </si>
+  <si>
+    <t>MYRGAL06_WM</t>
+  </si>
+  <si>
+    <t>BETALL09_SH</t>
+  </si>
+  <si>
+    <t>SAMRAC08_GR</t>
+  </si>
+  <si>
+    <t>SAMRAC09_GR</t>
+  </si>
+  <si>
+    <t>SAMRAC01_GR</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 10</t>
+  </si>
+  <si>
+    <t>SORAME_SH (plot 10)</t>
+  </si>
+  <si>
+    <t>SORAME01_SH</t>
+  </si>
+  <si>
+    <t>DIELONXX_GR</t>
+  </si>
+  <si>
+    <t>in GH5, according to Kea's email; replaces dead 1 in plot 10</t>
+  </si>
+  <si>
+    <t>replace dead one in plot 6 (I would add an extra one but we do not have it)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,6 +579,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +608,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -455,13 +664,90 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -489,6 +775,43 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -516,6 +839,43 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -856,7 +1216,7 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,8 +1232,11 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -890,7 +1253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -907,7 +1270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -924,7 +1287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -941,7 +1304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -958,7 +1321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -975,7 +1338,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -992,7 +1355,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1009,7 +1372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1043,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1423,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1077,7 +1440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1094,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1111,7 +1474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1162,7 +1525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1179,9 +1542,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1195,10 +1558,13 @@
       <c r="E20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1207,18 +1573,18 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -1230,7 +1596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1247,7 +1613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1264,7 +1630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1281,15 +1647,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1298,12 +1664,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -1312,106 +1678,118 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
       <c r="E32" t="s">
         <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -1419,16 +1797,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1436,10 +1814,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -1448,32 +1826,32 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
@@ -1482,12 +1860,12 @@
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -1499,12 +1877,12 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -1513,15 +1891,15 @@
         <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -1530,24 +1908,24 @@
         <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>21</v>
+      <c r="D41" t="s">
+        <v>8</v>
       </c>
       <c r="E41" t="s">
         <v>86</v>
@@ -1555,16 +1933,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
         <v>86</v>
@@ -1572,16 +1950,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
         <v>86</v>
@@ -1589,13 +1967,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -1606,33 +1984,33 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E45" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" t="s">
-        <v>8</v>
+      <c r="A46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E46" t="s">
         <v>86</v>
@@ -1640,19 +2018,19 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1669,15 +2047,15 @@
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
       </c>
       <c r="C49" t="s">
         <v>39</v>
@@ -1686,49 +2064,49 @@
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
       </c>
       <c r="C50" t="s">
         <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
       </c>
       <c r="C52" t="s">
         <v>39</v>
@@ -1742,7 +2120,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -1751,7 +2129,7 @@
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -1759,7 +2137,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -1768,7 +2146,7 @@
         <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -1776,16 +2154,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
       </c>
       <c r="C55" t="s">
         <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -1793,16 +2171,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -1810,16 +2188,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -1844,7 +2222,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -1853,15 +2231,15 @@
         <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -1870,58 +2248,58 @@
         <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>90</v>
-      </c>
-      <c r="B61" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
       </c>
       <c r="D61" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>89</v>
-      </c>
-      <c r="B62" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -1929,109 +2307,109 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
         <v>50</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B69" t="s">
         <v>9</v>
-      </c>
-      <c r="C64" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="C65" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67">
-        <v>4</v>
-      </c>
-      <c r="C67" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68">
-        <v>5</v>
-      </c>
-      <c r="C68" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69">
-        <v>3</v>
       </c>
       <c r="C69" t="s">
         <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E69" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -2040,21 +2418,21 @@
         <v>47</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E70" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -2063,32 +2441,32 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B73">
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -2097,32 +2475,32 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E74" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B75">
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
@@ -2131,66 +2509,75 @@
         <v>86</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>56</v>
-      </c>
-      <c r="B76">
+        <v>151</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77">
         <v>4</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" t="s">
+        <v>86</v>
+      </c>
+      <c r="F78" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
         <v>55</v>
-      </c>
-      <c r="D76" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77">
-        <v>5</v>
-      </c>
-      <c r="C77" t="s">
-        <v>61</v>
-      </c>
-      <c r="D77" t="s">
-        <v>21</v>
-      </c>
-      <c r="E77" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78">
-        <v>5</v>
-      </c>
-      <c r="C78" t="s">
-        <v>61</v>
-      </c>
-      <c r="D78" t="s">
-        <v>21</v>
-      </c>
-      <c r="E78" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" t="s">
-        <v>62</v>
-      </c>
-      <c r="B79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C79" t="s">
-        <v>61</v>
       </c>
       <c r="D79" t="s">
         <v>6</v>
@@ -2199,15 +2586,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D80" t="s">
         <v>6</v>
@@ -2216,15 +2603,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>65</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
@@ -2233,15 +2620,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
@@ -2250,117 +2637,120 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B83">
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D83" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E83" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>69</v>
-      </c>
-      <c r="B84" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="B84">
+        <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D84" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E85" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B86">
         <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E86" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>71</v>
-      </c>
-      <c r="B88">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -2369,32 +2759,32 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>78</v>
-      </c>
-      <c r="B90">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E90" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B91">
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
@@ -2403,191 +2793,499 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D92" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E92" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>74</v>
-      </c>
-      <c r="B93">
-        <v>5</v>
+        <v>69</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D93" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E93" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B94">
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F94" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>73</v>
+      </c>
+      <c r="B95">
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="C96" t="s">
+        <v>68</v>
+      </c>
+      <c r="D96" t="s">
         <v>8</v>
       </c>
-      <c r="E94" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" t="s">
-        <v>9</v>
-      </c>
-      <c r="C95" t="s">
-        <v>81</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E96" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>71</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+      <c r="C97" t="s">
+        <v>68</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>168</v>
+      </c>
+      <c r="C98" t="s">
+        <v>68</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" t="s">
         <v>6</v>
       </c>
-      <c r="E95" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" t="s">
-        <v>80</v>
-      </c>
-      <c r="B96" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" t="s">
-        <v>81</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E99" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>134</v>
+      </c>
+      <c r="C100" t="s">
+        <v>68</v>
+      </c>
+      <c r="D100" t="s">
         <v>6</v>
       </c>
-      <c r="E96" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" t="s">
-        <v>82</v>
-      </c>
-      <c r="B97" t="s">
-        <v>9</v>
-      </c>
-      <c r="C97" t="s">
-        <v>81</v>
-      </c>
-      <c r="D97" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" t="s">
-        <v>82</v>
-      </c>
-      <c r="B98" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" t="s">
-        <v>83</v>
-      </c>
-      <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" t="s">
-        <v>84</v>
-      </c>
-      <c r="D99" t="s">
-        <v>21</v>
-      </c>
-      <c r="E99" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" t="s">
-        <v>83</v>
-      </c>
-      <c r="B100" t="s">
-        <v>9</v>
-      </c>
-      <c r="C100" t="s">
-        <v>84</v>
-      </c>
-      <c r="D100" t="s">
-        <v>21</v>
-      </c>
       <c r="E100" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F100" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>85</v>
-      </c>
-      <c r="B101" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C101" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
       </c>
       <c r="E101" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F101" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>85</v>
-      </c>
-      <c r="B102" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
       </c>
       <c r="E102" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>76</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>45</v>
+      </c>
+      <c r="D103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>78</v>
+      </c>
+      <c r="B104">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
+        <v>45</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>75</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>45</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>77</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>45</v>
+      </c>
+      <c r="D106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>74</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>45</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>45</v>
+      </c>
+      <c r="D108" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" t="s">
+        <v>81</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>81</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>82</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" t="s">
+        <v>81</v>
+      </c>
+      <c r="D111" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>82</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" t="s">
+        <v>81</v>
+      </c>
+      <c r="D112" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" t="s">
+        <v>83</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" t="s">
+        <v>84</v>
+      </c>
+      <c r="D113" t="s">
+        <v>21</v>
+      </c>
+      <c r="E113" t="s">
+        <v>94</v>
+      </c>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" t="s">
+        <v>83</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" t="s">
+        <v>84</v>
+      </c>
+      <c r="D114" t="s">
+        <v>21</v>
+      </c>
+      <c r="E114" t="s">
+        <v>94</v>
+      </c>
+      <c r="J114" s="4"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" t="s">
+        <v>85</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" t="s">
+        <v>84</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>94</v>
+      </c>
+      <c r="J115" s="4"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" t="s">
+        <v>85</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" t="s">
+        <v>84</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
+        <v>94</v>
+      </c>
+      <c r="J116" s="4"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" t="s">
+        <v>156</v>
+      </c>
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s">
+        <v>157</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" t="s">
+        <v>13</v>
+      </c>
+      <c r="F117" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" t="s">
+        <v>156</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s">
+        <v>157</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" t="s">
+        <v>13</v>
+      </c>
+      <c r="F118" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>156</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>157</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>13</v>
+      </c>
+      <c r="F119" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2603,13 +3301,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2617,7 +3320,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2627,12 +3330,12 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2642,52 +3345,338 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="B36" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>